<commit_message>
add time elapse test
</commit_message>
<xml_diff>
--- a/trace.xlsx
+++ b/trace.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
   <si>
-    <t xml:space="preserve">a^2 + b * c = d
+    <t xml:space="preserve">2*(a^2 + b * c) = d
 a: 10
 b: 5
 c: 3
@@ -1255,7 +1255,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="7"/>
@@ -1265,7 +1265,7 @@
     <col min="8" max="8" width="55.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="127" customHeight="1" spans="1:8">
+    <row r="1" ht="141" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>